<commit_message>
fix OBV unit tests
</commit_message>
<xml_diff>
--- a/tests/indicators/m-r/Obv/Obv.Calc.xlsx
+++ b/tests/indicators/m-r/Obv/Obv.Calc.xlsx
@@ -1,25 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9F338C-3888-4D83-A0BF-C4232ADFF089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EED718-1BA2-4368-8895-02CCA5412A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22755" yWindow="1470" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OBV" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -565,7 +557,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1184,7 +1176,7 @@
   <dimension ref="A1:J503"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,7 +1245,9 @@
         <v>96708880</v>
       </c>
       <c r="H2" s="9"/>
-      <c r="I2" s="1"/>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
       <c r="J2" s="9"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1862,7 +1856,10 @@
         <f>IF(testdata[[#This Row],[upDown]]&gt;0,I20+testdata[[#This Row],[volume]],IF(testdata[[#This Row],[upDown]]&lt;0,I20-testdata[[#This Row],[volume]],I20))</f>
         <v>-25420052</v>
       </c>
-      <c r="J21" s="9"/>
+      <c r="J21" s="9">
+        <f>AVERAGE(I2:I21)</f>
+        <v>81233498</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6">

</xml_diff>

<commit_message>
feat: Full chain streaming prototypes (#1092)
Signed-off-by: Dave Skender <8432125+DaveSkender@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tests/indicators/m-r/Obv/Obv.Calc.xlsx
+++ b/tests/indicators/m-r/Obv/Obv.Calc.xlsx
@@ -1,25 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9F338C-3888-4D83-A0BF-C4232ADFF089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EED718-1BA2-4368-8895-02CCA5412A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22755" yWindow="1470" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OBV" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -565,7 +557,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1184,7 +1176,7 @@
   <dimension ref="A1:J503"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,7 +1245,9 @@
         <v>96708880</v>
       </c>
       <c r="H2" s="9"/>
-      <c r="I2" s="1"/>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
       <c r="J2" s="9"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1862,7 +1856,10 @@
         <f>IF(testdata[[#This Row],[upDown]]&gt;0,I20+testdata[[#This Row],[volume]],IF(testdata[[#This Row],[upDown]]&lt;0,I20-testdata[[#This Row],[volume]],I20))</f>
         <v>-25420052</v>
       </c>
-      <c r="J21" s="9"/>
+      <c r="J21" s="9">
+        <f>AVERAGE(I2:I21)</f>
+        <v>81233498</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6">

</xml_diff>